<commit_message>
admin view working and nice (without header stuff)
</commit_message>
<xml_diff>
--- a/resultFile/result.xlsx
+++ b/resultFile/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="24">
   <si>
     <t>Departure city</t>
   </si>
@@ -38,6 +38,54 @@
   </si>
   <si>
     <t>Fully bookedDate obtained</t>
+  </si>
+  <si>
+    <t>Łódź</t>
+  </si>
+  <si>
+    <t>Kraków</t>
+  </si>
+  <si>
+    <t>05.02.2020</t>
+  </si>
+  <si>
+    <t>00:30</t>
+  </si>
+  <si>
+    <t>04:00</t>
+  </si>
+  <si>
+    <t>06.01.2020 (20:08)</t>
+  </si>
+  <si>
+    <t>07:05</t>
+  </si>
+  <si>
+    <t>11:25</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>16:00</t>
+  </si>
+  <si>
+    <t>15:10</t>
+  </si>
+  <si>
+    <t>19:25</t>
+  </si>
+  <si>
+    <t>23:59</t>
+  </si>
+  <si>
+    <t>04:15</t>
+  </si>
+  <si>
+    <t>03.02.2020</t>
+  </si>
+  <si>
+    <t>04.02.2020</t>
   </si>
 </sst>
 </file>
@@ -369,13 +417,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,6 +447,470 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>29.99</v>
+      </c>
+      <c r="G2">
+        <v>0.12</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>45.99</v>
+      </c>
+      <c r="G3">
+        <v>0.184</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>39.99</v>
+      </c>
+      <c r="G4">
+        <v>0.16</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>39.99</v>
+      </c>
+      <c r="G5">
+        <v>0.16</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>29.99</v>
+      </c>
+      <c r="G6">
+        <v>0.12</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>29.99</v>
+      </c>
+      <c r="G7">
+        <v>0.12</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>39.99</v>
+      </c>
+      <c r="G8">
+        <v>0.16</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>39.99</v>
+      </c>
+      <c r="G9">
+        <v>0.16</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>39.99</v>
+      </c>
+      <c r="G10">
+        <v>0.16</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11">
+        <v>39.99</v>
+      </c>
+      <c r="G11">
+        <v>0.16</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>29.99</v>
+      </c>
+      <c r="G12">
+        <v>0.12</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>29.99</v>
+      </c>
+      <c r="G13">
+        <v>0.12</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>29.99</v>
+      </c>
+      <c r="G14">
+        <v>0.12</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>39.99</v>
+      </c>
+      <c r="G15">
+        <v>0.16</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16">
+        <v>39.99</v>
+      </c>
+      <c r="G16">
+        <v>0.16</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>29.99</v>
+      </c>
+      <c r="G17">
+        <v>0.12</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Usunięte śmieci z kodu. Proszę sprawdź komentarze z wykrzyknikami w webapp.py -> jest troche rzeczy do sprawdzenia
</commit_message>
<xml_diff>
--- a/resultFile/result.xlsx
+++ b/resultFile/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Departure city</t>
   </si>
@@ -37,7 +37,10 @@
     <t>Price per km</t>
   </si>
   <si>
-    <t>Fully bookedDate obtained</t>
+    <t>Fully booked</t>
+  </si>
+  <si>
+    <t>Date obtained</t>
   </si>
   <si>
     <t>Gdańsk</t>
@@ -421,22 +424,25 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>109.99</v>
@@ -448,24 +454,24 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <v>109.99</v>
@@ -477,7 +483,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
poprawienie błędu w zapytaniu z results. poprawiony błąd z czysczeniem bazy
</commit_message>
<xml_diff>
--- a/resultFile/result.xlsx
+++ b/resultFile/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="26">
   <si>
     <t>Departure city</t>
   </si>
@@ -37,31 +37,61 @@
     <t>Price per km</t>
   </si>
   <si>
-    <t>Fully booked</t>
-  </si>
-  <si>
-    <t>Date obtained</t>
-  </si>
-  <si>
-    <t>Gdańsk</t>
+    <t>Fully bookedDate obtained</t>
   </si>
   <si>
     <t>Kraków</t>
   </si>
   <si>
-    <t>02.02.2020</t>
-  </si>
-  <si>
-    <t>00:30</t>
-  </si>
-  <si>
-    <t>09:35</t>
-  </si>
-  <si>
-    <t>06.01.2020 (23:03)</t>
-  </si>
-  <si>
-    <t>06.01.2020 (23:06)</t>
+    <t>Łódź</t>
+  </si>
+  <si>
+    <t>20.01.2020</t>
+  </si>
+  <si>
+    <t>01:45</t>
+  </si>
+  <si>
+    <t>06:00</t>
+  </si>
+  <si>
+    <t>11.01.2020 (17:23)</t>
+  </si>
+  <si>
+    <t>02:00</t>
+  </si>
+  <si>
+    <t>05:30</t>
+  </si>
+  <si>
+    <t>02:20</t>
+  </si>
+  <si>
+    <t>07:00</t>
+  </si>
+  <si>
+    <t>09:05</t>
+  </si>
+  <si>
+    <t>13:15</t>
+  </si>
+  <si>
+    <t>13:05</t>
+  </si>
+  <si>
+    <t>17:05</t>
+  </si>
+  <si>
+    <t>18:20</t>
+  </si>
+  <si>
+    <t>22:40</t>
+  </si>
+  <si>
+    <t>21.01.2020</t>
+  </si>
+  <si>
+    <t>22.01.2020</t>
   </si>
 </sst>
 </file>
@@ -393,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -424,66 +454,1223 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2">
-        <v>109.99</v>
+        <v>29.99</v>
       </c>
       <c r="G2">
-        <v>0.7333</v>
+        <v>0.12</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.28</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="G4">
+        <v>0.28</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>45.99</v>
+      </c>
+      <c r="G5">
+        <v>0.184</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>39.99</v>
+      </c>
+      <c r="G6">
+        <v>0.16</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>39.99</v>
+      </c>
+      <c r="G7">
+        <v>0.16</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3">
-        <v>109.99</v>
-      </c>
-      <c r="G3">
-        <v>0.7333</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="F8">
+        <v>25.99</v>
+      </c>
+      <c r="G8">
+        <v>0.104</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
         <v>15</v>
+      </c>
+      <c r="F9">
+        <v>45.99</v>
+      </c>
+      <c r="G9">
+        <v>0.184</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="G10">
+        <v>0.28</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>25.99</v>
+      </c>
+      <c r="G11">
+        <v>0.104</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>45.99</v>
+      </c>
+      <c r="G12">
+        <v>0.184</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="G13">
+        <v>0.28</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14">
+        <v>39.99</v>
+      </c>
+      <c r="G14">
+        <v>0.16</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15">
+        <v>39.99</v>
+      </c>
+      <c r="G15">
+        <v>0.16</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16">
+        <v>39.99</v>
+      </c>
+      <c r="G16">
+        <v>0.16</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>55.99</v>
+      </c>
+      <c r="G17">
+        <v>0.224</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <v>55.99</v>
+      </c>
+      <c r="G18">
+        <v>0.224</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19">
+        <v>45.99</v>
+      </c>
+      <c r="G19">
+        <v>0.184</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20">
+        <v>49.99</v>
+      </c>
+      <c r="G20">
+        <v>0.2</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21">
+        <v>39.99</v>
+      </c>
+      <c r="G21">
+        <v>0.16</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <v>55.99</v>
+      </c>
+      <c r="G22">
+        <v>0.224</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>29.99</v>
+      </c>
+      <c r="G23">
+        <v>0.12</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.28</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="G25">
+        <v>0.28</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26">
+        <v>45.99</v>
+      </c>
+      <c r="G26">
+        <v>0.184</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27">
+        <v>39.99</v>
+      </c>
+      <c r="G27">
+        <v>0.16</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28">
+        <v>39.99</v>
+      </c>
+      <c r="G28">
+        <v>0.16</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>25.99</v>
+      </c>
+      <c r="G29">
+        <v>0.104</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>45.99</v>
+      </c>
+      <c r="G30">
+        <v>0.184</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="G31">
+        <v>0.28</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>25.99</v>
+      </c>
+      <c r="G32">
+        <v>0.104</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33">
+        <v>45.99</v>
+      </c>
+      <c r="G33">
+        <v>0.184</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="G34">
+        <v>0.28</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35">
+        <v>39.99</v>
+      </c>
+      <c r="G35">
+        <v>0.16</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36">
+        <v>39.99</v>
+      </c>
+      <c r="G36">
+        <v>0.16</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37">
+        <v>39.99</v>
+      </c>
+      <c r="G37">
+        <v>0.16</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38">
+        <v>55.99</v>
+      </c>
+      <c r="G38">
+        <v>0.224</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39">
+        <v>55.99</v>
+      </c>
+      <c r="G39">
+        <v>0.224</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40">
+        <v>45.99</v>
+      </c>
+      <c r="G40">
+        <v>0.184</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41">
+        <v>49.99</v>
+      </c>
+      <c r="G41">
+        <v>0.2</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42">
+        <v>39.99</v>
+      </c>
+      <c r="G42">
+        <v>0.16</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43">
+        <v>55.99</v>
+      </c>
+      <c r="G43">
+        <v>0.224</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Poprawiony view job results - był zły tytuł
</commit_message>
<xml_diff>
--- a/resultFile/result.xlsx
+++ b/resultFile/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="27">
   <si>
     <t>Departure city</t>
   </si>
@@ -40,58 +40,61 @@
     <t>Fully bookedDate obtained</t>
   </si>
   <si>
-    <t>Kraków</t>
+    <t>Szczecin</t>
   </si>
   <si>
-    <t>Łódź</t>
+    <t>Poznań</t>
   </si>
   <si>
-    <t>20.01.2020</t>
+    <t>23.01.2020</t>
   </si>
   <si>
-    <t>01:45</t>
+    <t>04:00</t>
   </si>
   <si>
-    <t>06:00</t>
+    <t>07:30</t>
   </si>
   <si>
-    <t>11.01.2020 (17:23)</t>
+    <t>11.01.2020 (17:33)</t>
   </si>
   <si>
-    <t>02:00</t>
+    <t>17:10</t>
   </si>
   <si>
-    <t>05:30</t>
+    <t>20:40</t>
   </si>
   <si>
-    <t>02:20</t>
+    <t>24.01.2020</t>
   </si>
   <si>
-    <t>07:00</t>
+    <t>25.01.2020</t>
   </si>
   <si>
-    <t>09:05</t>
+    <t>26.01.2020</t>
   </si>
   <si>
-    <t>13:15</t>
+    <t>27.01.2020</t>
   </si>
   <si>
-    <t>13:05</t>
+    <t>28.01.2020</t>
   </si>
   <si>
-    <t>17:05</t>
+    <t>29.01.2020</t>
   </si>
   <si>
-    <t>18:20</t>
+    <t>30.01.2020</t>
   </si>
   <si>
-    <t>22:40</t>
+    <t>31.01.2020</t>
   </si>
   <si>
-    <t>21.01.2020</t>
+    <t>11.01.2020 (17:34)</t>
   </si>
   <si>
-    <t>22.01.2020</t>
+    <t>11.01.2020 (17:37)</t>
+  </si>
+  <si>
+    <t>11.01.2020 (17:38)</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -472,10 +475,7 @@
         <v>12</v>
       </c>
       <c r="F2">
-        <v>29.99</v>
-      </c>
-      <c r="G2">
-        <v>0.12</v>
+        <v>25.99</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -501,10 +501,7 @@
         <v>15</v>
       </c>
       <c r="F3">
-        <v>69.98999999999999</v>
-      </c>
-      <c r="G3">
-        <v>0.28</v>
+        <v>14.99</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -524,16 +521,13 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F4">
-        <v>69.98999999999999</v>
-      </c>
-      <c r="G4">
-        <v>0.28</v>
+        <v>29.99</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -550,19 +544,16 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>45.99</v>
-      </c>
-      <c r="G5">
-        <v>0.184</v>
+        <v>29.99</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -579,19 +570,16 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F6">
-        <v>39.99</v>
-      </c>
-      <c r="G6">
-        <v>0.16</v>
+        <v>35.99</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -608,19 +596,16 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>39.99</v>
-      </c>
-      <c r="G7">
-        <v>0.16</v>
+        <v>35.99</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -637,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -646,10 +631,7 @@
         <v>12</v>
       </c>
       <c r="F8">
-        <v>25.99</v>
-      </c>
-      <c r="G8">
-        <v>0.104</v>
+        <v>35.99</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -666,7 +648,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -675,10 +657,7 @@
         <v>15</v>
       </c>
       <c r="F9">
-        <v>45.99</v>
-      </c>
-      <c r="G9">
-        <v>0.184</v>
+        <v>35.99</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -695,19 +674,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F10">
-        <v>69.98999999999999</v>
-      </c>
-      <c r="G10">
-        <v>0.28</v>
+        <v>14.99</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -724,7 +700,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -733,10 +709,7 @@
         <v>12</v>
       </c>
       <c r="F11">
-        <v>25.99</v>
-      </c>
-      <c r="G11">
-        <v>0.104</v>
+        <v>14.99</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -753,7 +726,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -762,10 +735,7 @@
         <v>15</v>
       </c>
       <c r="F12">
-        <v>45.99</v>
-      </c>
-      <c r="G12">
-        <v>0.184</v>
+        <v>29.99</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -782,19 +752,16 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F13">
-        <v>69.98999999999999</v>
-      </c>
-      <c r="G13">
-        <v>0.28</v>
+        <v>29.99</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -811,19 +778,16 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F14">
-        <v>39.99</v>
-      </c>
-      <c r="G14">
-        <v>0.16</v>
+        <v>29.99</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -840,19 +804,16 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F15">
-        <v>39.99</v>
-      </c>
-      <c r="G15">
-        <v>0.16</v>
+        <v>25.99</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -869,19 +830,16 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F16">
-        <v>39.99</v>
-      </c>
-      <c r="G16">
-        <v>0.16</v>
+        <v>35.99</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -898,19 +856,16 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F17">
-        <v>55.99</v>
-      </c>
-      <c r="G17">
-        <v>0.224</v>
+        <v>35.99</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -927,7 +882,7 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -936,10 +891,7 @@
         <v>15</v>
       </c>
       <c r="F18">
-        <v>55.99</v>
-      </c>
-      <c r="G18">
-        <v>0.224</v>
+        <v>14.99</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -956,19 +908,16 @@
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F19">
-        <v>45.99</v>
-      </c>
-      <c r="G19">
-        <v>0.184</v>
+        <v>29.99</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -985,19 +934,16 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F20">
-        <v>49.99</v>
-      </c>
-      <c r="G20">
-        <v>0.2</v>
+        <v>29.99</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1014,19 +960,16 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F21">
-        <v>39.99</v>
-      </c>
-      <c r="G21">
-        <v>0.16</v>
+        <v>14.99</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1043,19 +986,16 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F22">
-        <v>55.99</v>
-      </c>
-      <c r="G22">
-        <v>0.224</v>
+        <v>29.99</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1072,7 +1012,7 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -1082,9 +1022,6 @@
       </c>
       <c r="F23">
         <v>29.99</v>
-      </c>
-      <c r="G23">
-        <v>0.12</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1101,7 +1038,7 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
@@ -1110,10 +1047,7 @@
         <v>15</v>
       </c>
       <c r="F24">
-        <v>69.98999999999999</v>
-      </c>
-      <c r="G24">
-        <v>0.28</v>
+        <v>14.99</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1130,19 +1064,16 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F25">
-        <v>69.98999999999999</v>
-      </c>
-      <c r="G25">
-        <v>0.28</v>
+        <v>35.99</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1159,19 +1090,16 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F26">
-        <v>45.99</v>
-      </c>
-      <c r="G26">
-        <v>0.184</v>
+        <v>35.99</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1188,19 +1116,16 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F27">
-        <v>39.99</v>
-      </c>
-      <c r="G27">
-        <v>0.16</v>
+        <v>29.99</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1217,19 +1142,16 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F28">
-        <v>39.99</v>
-      </c>
-      <c r="G28">
-        <v>0.16</v>
+        <v>29.99</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1257,14 +1179,11 @@
       <c r="F29">
         <v>25.99</v>
       </c>
-      <c r="G29">
-        <v>0.104</v>
-      </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1284,16 +1203,13 @@
         <v>15</v>
       </c>
       <c r="F30">
-        <v>45.99</v>
-      </c>
-      <c r="G30">
-        <v>0.184</v>
+        <v>14.99</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1307,22 +1223,19 @@
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F31">
-        <v>69.98999999999999</v>
-      </c>
-      <c r="G31">
-        <v>0.28</v>
+        <v>29.99</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1333,25 +1246,22 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>29.99</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
         <v>24</v>
-      </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32">
-        <v>25.99</v>
-      </c>
-      <c r="G32">
-        <v>0.104</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1362,25 +1272,22 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33">
+        <v>35.99</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
         <v>24</v>
-      </c>
-      <c r="D33" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33">
-        <v>45.99</v>
-      </c>
-      <c r="G33">
-        <v>0.184</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1391,25 +1298,22 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34">
+        <v>35.99</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
         <v>24</v>
-      </c>
-      <c r="D34" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34">
-        <v>69.98999999999999</v>
-      </c>
-      <c r="G34">
-        <v>0.28</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1420,25 +1324,22 @@
         <v>9</v>
       </c>
       <c r="C35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>35.99</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
         <v>24</v>
-      </c>
-      <c r="D35" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35">
-        <v>39.99</v>
-      </c>
-      <c r="G35">
-        <v>0.16</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1449,25 +1350,22 @@
         <v>9</v>
       </c>
       <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <v>35.99</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
         <v>24</v>
-      </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36">
-        <v>39.99</v>
-      </c>
-      <c r="G36">
-        <v>0.16</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1478,25 +1376,22 @@
         <v>9</v>
       </c>
       <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37">
+        <v>14.99</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
         <v>24</v>
-      </c>
-      <c r="D37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" t="s">
-        <v>23</v>
-      </c>
-      <c r="F37">
-        <v>39.99</v>
-      </c>
-      <c r="G37">
-        <v>0.16</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1507,25 +1402,22 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38">
+        <v>14.99</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
         <v>24</v>
-      </c>
-      <c r="D38" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38">
-        <v>55.99</v>
-      </c>
-      <c r="G38">
-        <v>0.224</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1536,7 +1428,7 @@
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
@@ -1545,16 +1437,13 @@
         <v>15</v>
       </c>
       <c r="F39">
-        <v>55.99</v>
-      </c>
-      <c r="G39">
-        <v>0.224</v>
+        <v>29.99</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1565,25 +1454,22 @@
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F40">
-        <v>45.99</v>
-      </c>
-      <c r="G40">
-        <v>0.184</v>
+        <v>29.99</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1594,25 +1480,22 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F41">
-        <v>49.99</v>
-      </c>
-      <c r="G41">
-        <v>0.2</v>
+        <v>29.99</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1623,25 +1506,22 @@
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F42">
-        <v>39.99</v>
-      </c>
-      <c r="G42">
-        <v>0.16</v>
+        <v>25.99</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1652,25 +1532,1660 @@
         <v>9</v>
       </c>
       <c r="C43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43">
+        <v>35.99</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44">
+        <v>35.99</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45">
+        <v>14.99</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46">
+        <v>29.99</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47">
+        <v>29.99</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48">
+        <v>14.99</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49">
+        <v>29.99</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50">
+        <v>29.99</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51">
+        <v>14.99</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52">
+        <v>35.99</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53">
+        <v>25.99</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
         <v>25</v>
       </c>
-      <c r="D43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43">
-        <v>55.99</v>
-      </c>
-      <c r="G43">
-        <v>0.224</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43" t="s">
-        <v>13</v>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54">
+        <v>14.99</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55">
+        <v>29.99</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56">
+        <v>29.99</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57">
+        <v>35.99</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58">
+        <v>35.99</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59">
+        <v>35.99</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60">
+        <v>35.99</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61">
+        <v>14.99</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62">
+        <v>14.99</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63">
+        <v>29.99</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64">
+        <v>29.99</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65">
+        <v>29.99</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>19</v>
+      </c>
+      <c r="D66" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66">
+        <v>25.99</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D67" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67">
+        <v>35.99</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68">
+        <v>35.99</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
+        <v>20</v>
+      </c>
+      <c r="D69" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69">
+        <v>14.99</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70">
+        <v>29.99</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71">
+        <v>29.99</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
+        <v>21</v>
+      </c>
+      <c r="D72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" t="s">
+        <v>15</v>
+      </c>
+      <c r="F72">
+        <v>14.99</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
+        <v>21</v>
+      </c>
+      <c r="D73" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73">
+        <v>29.99</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" t="s">
+        <v>22</v>
+      </c>
+      <c r="D74" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74">
+        <v>29.99</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" t="s">
+        <v>22</v>
+      </c>
+      <c r="D75" t="s">
+        <v>14</v>
+      </c>
+      <c r="E75" t="s">
+        <v>15</v>
+      </c>
+      <c r="F75">
+        <v>14.99</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76">
+        <v>35.99</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77">
+        <v>35.99</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78">
+        <v>29.99</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79">
+        <v>29.99</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" t="s">
+        <v>10</v>
+      </c>
+      <c r="D80" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80">
+        <v>25.99</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81" t="s">
+        <v>14</v>
+      </c>
+      <c r="E81" t="s">
+        <v>15</v>
+      </c>
+      <c r="F81">
+        <v>14.99</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82">
+        <v>29.99</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" t="s">
+        <v>12</v>
+      </c>
+      <c r="F83">
+        <v>29.99</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" t="s">
+        <v>14</v>
+      </c>
+      <c r="E84" t="s">
+        <v>15</v>
+      </c>
+      <c r="F84">
+        <v>35.99</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85">
+        <v>35.99</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86">
+        <v>35.99</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" t="s">
+        <v>17</v>
+      </c>
+      <c r="D87" t="s">
+        <v>14</v>
+      </c>
+      <c r="E87" t="s">
+        <v>15</v>
+      </c>
+      <c r="F87">
+        <v>35.99</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" t="s">
+        <v>17</v>
+      </c>
+      <c r="D88" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88">
+        <v>14.99</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89">
+        <v>14.99</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" t="s">
+        <v>18</v>
+      </c>
+      <c r="D90" t="s">
+        <v>14</v>
+      </c>
+      <c r="E90" t="s">
+        <v>15</v>
+      </c>
+      <c r="F90">
+        <v>29.99</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91">
+        <v>29.99</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" t="s">
+        <v>19</v>
+      </c>
+      <c r="D92" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92">
+        <v>29.99</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" t="s">
+        <v>19</v>
+      </c>
+      <c r="D93" t="s">
+        <v>14</v>
+      </c>
+      <c r="E93" t="s">
+        <v>15</v>
+      </c>
+      <c r="F93">
+        <v>25.99</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94" t="s">
+        <v>19</v>
+      </c>
+      <c r="D94" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94">
+        <v>35.99</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" t="s">
+        <v>20</v>
+      </c>
+      <c r="D95" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95">
+        <v>35.99</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" t="s">
+        <v>20</v>
+      </c>
+      <c r="D96" t="s">
+        <v>14</v>
+      </c>
+      <c r="E96" t="s">
+        <v>15</v>
+      </c>
+      <c r="F96">
+        <v>14.99</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" t="s">
+        <v>20</v>
+      </c>
+      <c r="D97" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97">
+        <v>29.99</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" t="s">
+        <v>11</v>
+      </c>
+      <c r="E98" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98">
+        <v>29.99</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" t="s">
+        <v>14</v>
+      </c>
+      <c r="E99" t="s">
+        <v>15</v>
+      </c>
+      <c r="F99">
+        <v>14.99</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" t="s">
+        <v>21</v>
+      </c>
+      <c r="D100" t="s">
+        <v>11</v>
+      </c>
+      <c r="E100" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100">
+        <v>29.99</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" t="s">
+        <v>8</v>
+      </c>
+      <c r="B101" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" t="s">
+        <v>11</v>
+      </c>
+      <c r="E101" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101">
+        <v>29.99</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102" t="s">
+        <v>22</v>
+      </c>
+      <c r="D102" t="s">
+        <v>14</v>
+      </c>
+      <c r="E102" t="s">
+        <v>15</v>
+      </c>
+      <c r="F102">
+        <v>14.99</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" t="s">
+        <v>22</v>
+      </c>
+      <c r="D103" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" t="s">
+        <v>12</v>
+      </c>
+      <c r="F103">
+        <v>35.99</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104" t="s">
+        <v>9</v>
+      </c>
+      <c r="C104" t="s">
+        <v>23</v>
+      </c>
+      <c r="D104" t="s">
+        <v>11</v>
+      </c>
+      <c r="E104" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104">
+        <v>35.99</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" t="s">
+        <v>23</v>
+      </c>
+      <c r="D105" t="s">
+        <v>14</v>
+      </c>
+      <c r="E105" t="s">
+        <v>15</v>
+      </c>
+      <c r="F105">
+        <v>29.99</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" t="s">
+        <v>8</v>
+      </c>
+      <c r="B106" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" t="s">
+        <v>23</v>
+      </c>
+      <c r="D106" t="s">
+        <v>11</v>
+      </c>
+      <c r="E106" t="s">
+        <v>12</v>
+      </c>
+      <c r="F106">
+        <v>29.99</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
repair password and db location
</commit_message>
<xml_diff>
--- a/resultFile/result.xlsx
+++ b/resultFile/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="27">
   <si>
     <t>Departure city</t>
   </si>
@@ -40,25 +40,61 @@
     <t>Fully bookedDate obtained</t>
   </si>
   <si>
-    <t>Gdańsk</t>
-  </si>
-  <si>
-    <t>Kraków</t>
-  </si>
-  <si>
-    <t>02.02.2020</t>
-  </si>
-  <si>
-    <t>00:30</t>
-  </si>
-  <si>
-    <t>09:35</t>
-  </si>
-  <si>
-    <t>11.01.2020 (17:34)</t>
-  </si>
-  <si>
-    <t>11.01.2020 (22:53)</t>
+    <t>Wrocław</t>
+  </si>
+  <si>
+    <t>Poznań</t>
+  </si>
+  <si>
+    <t>20.01.2020</t>
+  </si>
+  <si>
+    <t>02:20</t>
+  </si>
+  <si>
+    <t>05:10</t>
+  </si>
+  <si>
+    <t>14.01.2020 (18:48)</t>
+  </si>
+  <si>
+    <t>04:20</t>
+  </si>
+  <si>
+    <t>07:10</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>10:35</t>
+  </si>
+  <si>
+    <t>13:45</t>
+  </si>
+  <si>
+    <t>16:20</t>
+  </si>
+  <si>
+    <t>18:15</t>
+  </si>
+  <si>
+    <t>20:50</t>
+  </si>
+  <si>
+    <t>19:45</t>
+  </si>
+  <si>
+    <t>22:35</t>
+  </si>
+  <si>
+    <t>21.01.2020</t>
+  </si>
+  <si>
+    <t>22.01.2020</t>
+  </si>
+  <si>
+    <t>23.01.2020</t>
   </si>
 </sst>
 </file>
@@ -390,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -439,10 +475,7 @@
         <v>12</v>
       </c>
       <c r="F2">
-        <v>129.99</v>
-      </c>
-      <c r="G2">
-        <v>0.8666</v>
+        <v>19.99</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -462,22 +495,695 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>19.99</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>27.99</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>27.99</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>19.99</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>19.99</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="F3">
-        <v>129.99</v>
-      </c>
-      <c r="G3">
-        <v>0.8666</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="F8">
+        <v>19.99</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>19.99</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
         <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>19.99</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>27.99</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12">
+        <v>19.99</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13">
+        <v>19.99</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14">
+        <v>19.99</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15">
+        <v>19.99</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <v>19.99</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>19.99</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>19.99</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19">
+        <v>19.99</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20">
+        <v>19.99</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21">
+        <v>19.99</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>19.99</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>19.99</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <v>19.99</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25">
+        <v>19.99</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26">
+        <v>27.99</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27">
+        <v>19.99</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28">
+        <v>19.99</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>19.99</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated presentation and database
</commit_message>
<xml_diff>
--- a/resultFile/result.xlsx
+++ b/resultFile/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="26">
   <si>
     <t>Departure city</t>
   </si>
@@ -40,67 +40,58 @@
     <t>Fully bookedDate obtained</t>
   </si>
   <si>
-    <t>Wrocław</t>
-  </si>
-  <si>
-    <t>Gdańsk</t>
-  </si>
-  <si>
-    <t>28.01.2020</t>
-  </si>
-  <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>18:55</t>
-  </si>
-  <si>
-    <t>14.01.2020 (19:14)</t>
-  </si>
-  <si>
-    <t>08:05</t>
-  </si>
-  <si>
-    <t>19:35</t>
-  </si>
-  <si>
-    <t>08:25</t>
-  </si>
-  <si>
-    <t>08:30</t>
-  </si>
-  <si>
-    <t>16:20</t>
-  </si>
-  <si>
-    <t>08:45</t>
-  </si>
-  <si>
-    <t>13:05</t>
-  </si>
-  <si>
-    <t>23:00</t>
-  </si>
-  <si>
-    <t>14:10</t>
-  </si>
-  <si>
-    <t>22:35</t>
-  </si>
-  <si>
-    <t>14:25</t>
-  </si>
-  <si>
-    <t>21:35</t>
-  </si>
-  <si>
-    <t>07:10</t>
-  </si>
-  <si>
-    <t>21:50</t>
-  </si>
-  <si>
-    <t>29.01.2020</t>
+    <t>Łódź</t>
+  </si>
+  <si>
+    <t>Kraków</t>
+  </si>
+  <si>
+    <t>05.02.2020</t>
+  </si>
+  <si>
+    <t>00:30</t>
+  </si>
+  <si>
+    <t>04:00</t>
+  </si>
+  <si>
+    <t>17.01.2020 (00:19)</t>
+  </si>
+  <si>
+    <t>07:05</t>
+  </si>
+  <si>
+    <t>11:25</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>16:00</t>
+  </si>
+  <si>
+    <t>15:10</t>
+  </si>
+  <si>
+    <t>19:25</t>
+  </si>
+  <si>
+    <t>23:59</t>
+  </si>
+  <si>
+    <t>04:15</t>
+  </si>
+  <si>
+    <t>03.02.2020</t>
+  </si>
+  <si>
+    <t>04.02.2020</t>
+  </si>
+  <si>
+    <t>17.01.2020 (00:20)</t>
+  </si>
+  <si>
+    <t>17.01.2020 (16:54)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -481,7 +472,10 @@
         <v>12</v>
       </c>
       <c r="F2">
-        <v>59.98</v>
+        <v>29.99</v>
+      </c>
+      <c r="G2">
+        <v>0.12</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -507,7 +501,10 @@
         <v>15</v>
       </c>
       <c r="F3">
-        <v>69.98</v>
+        <v>45.99</v>
+      </c>
+      <c r="G3">
+        <v>0.184</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -530,10 +527,13 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4">
-        <v>69.98</v>
+        <v>45.99</v>
+      </c>
+      <c r="G4">
+        <v>0.184</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -553,13 +553,16 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>39.99</v>
+      </c>
+      <c r="G5">
+        <v>0.16</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -579,13 +582,16 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F6">
-        <v>39.99</v>
+        <v>29.99</v>
+      </c>
+      <c r="G6">
+        <v>0.12</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -605,13 +611,16 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>99.98</v>
+        <v>29.99</v>
+      </c>
+      <c r="G7">
+        <v>0.12</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -628,16 +637,19 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F8">
-        <v>35.99</v>
+        <v>39.99</v>
+      </c>
+      <c r="G8">
+        <v>0.16</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -654,16 +666,19 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F9">
-        <v>35.99</v>
+        <v>39.99</v>
+      </c>
+      <c r="G9">
+        <v>0.16</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -680,16 +695,19 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F10">
-        <v>45.98</v>
+        <v>39.99</v>
+      </c>
+      <c r="G10">
+        <v>0.16</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -706,16 +724,19 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F11">
-        <v>45.98</v>
+        <v>39.99</v>
+      </c>
+      <c r="G11">
+        <v>0.16</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -732,7 +753,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -741,7 +762,10 @@
         <v>12</v>
       </c>
       <c r="F12">
-        <v>69.98</v>
+        <v>39.99</v>
+      </c>
+      <c r="G12">
+        <v>0.16</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -758,16 +782,19 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F13">
-        <v>69.98</v>
+        <v>39.99</v>
+      </c>
+      <c r="G13">
+        <v>0.16</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -784,16 +811,19 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
       </c>
       <c r="F14">
-        <v>69.98</v>
+        <v>29.99</v>
+      </c>
+      <c r="G14">
+        <v>0.12</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -810,16 +840,19 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
         <v>17</v>
       </c>
-      <c r="E15" t="s">
-        <v>18</v>
-      </c>
       <c r="F15">
         <v>39.99</v>
+      </c>
+      <c r="G15">
+        <v>0.16</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -836,16 +869,19 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
         <v>19</v>
       </c>
-      <c r="E16" t="s">
-        <v>18</v>
-      </c>
       <c r="F16">
         <v>39.99</v>
+      </c>
+      <c r="G16">
+        <v>0.16</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -862,16 +898,19 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F17">
-        <v>79.98</v>
+        <v>29.99</v>
+      </c>
+      <c r="G17">
+        <v>0.12</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -888,16 +927,19 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F18">
-        <v>39.99</v>
+        <v>29.99</v>
+      </c>
+      <c r="G18">
+        <v>0.12</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -914,16 +956,19 @@
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F19">
-        <v>39.99</v>
+        <v>45.99</v>
+      </c>
+      <c r="G19">
+        <v>0.184</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -940,16 +985,19 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F20">
-        <v>45.98</v>
+        <v>45.99</v>
+      </c>
+      <c r="G20">
+        <v>0.184</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -966,22 +1014,1301 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F21">
-        <v>45.98</v>
+        <v>39.99</v>
+      </c>
+      <c r="G21">
+        <v>0.16</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <v>29.99</v>
+      </c>
+      <c r="G22">
+        <v>0.12</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>29.99</v>
+      </c>
+      <c r="G23">
+        <v>0.12</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>39.99</v>
+      </c>
+      <c r="G24">
+        <v>0.16</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>39.99</v>
+      </c>
+      <c r="G25">
+        <v>0.16</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26">
+        <v>39.99</v>
+      </c>
+      <c r="G26">
+        <v>0.16</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27">
+        <v>39.99</v>
+      </c>
+      <c r="G27">
+        <v>0.16</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28">
+        <v>39.99</v>
+      </c>
+      <c r="G28">
+        <v>0.16</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>39.99</v>
+      </c>
+      <c r="G29">
+        <v>0.16</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>29.99</v>
+      </c>
+      <c r="G30">
+        <v>0.12</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31">
+        <v>39.99</v>
+      </c>
+      <c r="G31">
+        <v>0.16</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32">
+        <v>39.99</v>
+      </c>
+      <c r="G32">
+        <v>0.16</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33">
+        <v>29.99</v>
+      </c>
+      <c r="G33">
+        <v>0.12</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34">
+        <v>29.99</v>
+      </c>
+      <c r="G34">
+        <v>0.12</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35">
+        <v>45.99</v>
+      </c>
+      <c r="G35">
+        <v>0.184</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36">
+        <v>45.99</v>
+      </c>
+      <c r="G36">
+        <v>0.184</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37">
+        <v>39.99</v>
+      </c>
+      <c r="G37">
+        <v>0.16</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38">
+        <v>29.99</v>
+      </c>
+      <c r="G38">
+        <v>0.12</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <v>29.99</v>
+      </c>
+      <c r="G39">
+        <v>0.12</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40">
+        <v>39.99</v>
+      </c>
+      <c r="G40">
+        <v>0.16</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41">
+        <v>39.99</v>
+      </c>
+      <c r="G41">
+        <v>0.16</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42">
+        <v>39.99</v>
+      </c>
+      <c r="G42">
+        <v>0.16</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43">
+        <v>39.99</v>
+      </c>
+      <c r="G43">
+        <v>0.16</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44">
+        <v>39.99</v>
+      </c>
+      <c r="G44">
+        <v>0.16</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45">
+        <v>39.99</v>
+      </c>
+      <c r="G45">
+        <v>0.16</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46">
+        <v>29.99</v>
+      </c>
+      <c r="G46">
+        <v>0.12</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47">
+        <v>39.99</v>
+      </c>
+      <c r="G47">
+        <v>0.16</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48">
+        <v>39.99</v>
+      </c>
+      <c r="G48">
+        <v>0.16</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49">
+        <v>29.99</v>
+      </c>
+      <c r="G49">
+        <v>0.12</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50">
+        <v>29.99</v>
+      </c>
+      <c r="G50">
+        <v>0.12</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51">
+        <v>45.99</v>
+      </c>
+      <c r="G51">
+        <v>0.184</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52">
+        <v>45.99</v>
+      </c>
+      <c r="G52">
+        <v>0.184</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53">
+        <v>39.99</v>
+      </c>
+      <c r="G53">
+        <v>0.16</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54">
+        <v>29.99</v>
+      </c>
+      <c r="G54">
+        <v>0.12</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55">
+        <v>29.99</v>
+      </c>
+      <c r="G55">
+        <v>0.12</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56">
+        <v>39.99</v>
+      </c>
+      <c r="G56">
+        <v>0.16</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57">
+        <v>39.99</v>
+      </c>
+      <c r="G57">
+        <v>0.16</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58">
+        <v>39.99</v>
+      </c>
+      <c r="G58">
+        <v>0.16</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59">
+        <v>39.99</v>
+      </c>
+      <c r="G59">
+        <v>0.16</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60">
+        <v>39.99</v>
+      </c>
+      <c r="G60">
+        <v>0.16</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61">
+        <v>39.99</v>
+      </c>
+      <c r="G61">
+        <v>0.16</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62" t="s">
+        <v>15</v>
+      </c>
+      <c r="F62">
+        <v>29.99</v>
+      </c>
+      <c r="G62">
+        <v>0.12</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63">
+        <v>39.99</v>
+      </c>
+      <c r="G63">
+        <v>0.16</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64">
+        <v>39.99</v>
+      </c>
+      <c r="G64">
+        <v>0.16</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65">
+        <v>29.99</v>
+      </c>
+      <c r="G65">
+        <v>0.12</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>